<commit_message>
removed column in cards.xlsx
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="206">
   <si>
     <t>Description</t>
   </si>
@@ -341,12 +341,6 @@
     </r>
   </si>
   <si>
-    <t>Level Available</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Acid Splash</t>
   </si>
   <si>
@@ -496,9 +490,6 @@
     <t>Attribute</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>STR</t>
   </si>
   <si>
@@ -2859,15 +2850,6 @@
       </rPr>
       <t>Inflict Wound. Exhaust.</t>
     </r>
-  </si>
-  <si>
-    <t>Starter Cards</t>
-  </si>
-  <si>
-    <t>Injuries</t>
-  </si>
-  <si>
-    <t>Racial Cards</t>
   </si>
   <si>
     <t>Feature Cards</t>
@@ -3515,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3527,11 +3509,10 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3539,22 +3520,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3565,19 +3543,16 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3588,19 +3563,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3611,19 +3583,16 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3634,19 +3603,16 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3654,22 +3620,19 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3677,22 +3640,19 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3700,22 +3660,19 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3723,22 +3680,19 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -3746,22 +3700,19 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -3769,22 +3720,19 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>204</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -3792,22 +3740,19 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>204</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3815,22 +3760,19 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3838,22 +3780,19 @@
         <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="E14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3861,45 +3800,39 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>198</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3907,45 +3840,39 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3953,68 +3880,59 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>205</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>199</v>
+      </c>
+      <c r="E19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -4022,68 +3940,59 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>205</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>199</v>
+      </c>
+      <c r="E22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D24" t="s">
-        <v>204</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>198</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -4094,19 +4003,16 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -4117,19 +4023,16 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -4140,20 +4043,17 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>208</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-      <c r="F27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -4164,20 +4064,17 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>208</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -4188,20 +4085,17 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -4212,20 +4106,17 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
-      </c>
-      <c r="E30">
-        <v>3</v>
-      </c>
-      <c r="F30" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -4236,20 +4127,17 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>208</v>
-      </c>
-      <c r="E31">
-        <v>3</v>
-      </c>
-      <c r="F31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -4260,20 +4148,17 @@
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>208</v>
-      </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -4284,20 +4169,17 @@
         <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -4308,20 +4190,17 @@
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>208</v>
-      </c>
-      <c r="E34">
-        <v>3</v>
-      </c>
-      <c r="F34" t="s">
-        <v>74</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -4332,20 +4211,17 @@
         <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>208</v>
-      </c>
-      <c r="E35">
-        <v>16</v>
-      </c>
-      <c r="F35" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -4356,20 +4232,17 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
-      </c>
-      <c r="E36">
-        <v>16</v>
-      </c>
-      <c r="F36" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -4380,20 +4253,17 @@
         <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E37">
-        <v>16</v>
-      </c>
-      <c r="F37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -4404,802 +4274,697 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>208</v>
-      </c>
-      <c r="E38">
-        <v>16</v>
-      </c>
-      <c r="F38" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8">
+        <v>202</v>
+      </c>
+      <c r="E38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D39" t="s">
-        <v>209</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>209</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>83</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D41" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>83</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D42" t="s">
-        <v>209</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>209</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>83</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
         <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44">
-        <v>3</v>
-      </c>
-      <c r="F44" t="s">
-        <v>83</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E44" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
-        <v>209</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>133</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D46" t="s">
-        <v>209</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E46" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>209</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>83</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>203</v>
+      </c>
+      <c r="E47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
         <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D48" t="s">
-        <v>209</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>83</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>209</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>83</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E49" t="s">
+        <v>80</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B50" t="s">
         <v>19</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>209</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>83</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
-        <v>209</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E51" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>205</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>73</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>199</v>
+      </c>
+      <c r="E52" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B53" t="s">
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>209</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>83</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E53" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B54" t="s">
         <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
-        <v>209</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>83</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D55" t="s">
-        <v>209</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" t="s">
+        <v>203</v>
+      </c>
+      <c r="E55" t="s">
+        <v>80</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
         <v>83</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>86</v>
       </c>
       <c r="B56" t="s">
         <v>19</v>
       </c>
       <c r="C56" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>209</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56" t="s">
-        <v>83</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E56" t="s">
+        <v>80</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" t="s">
-        <v>83</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E57" t="s">
+        <v>80</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B58" t="s">
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" t="s">
-        <v>133</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E59" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D60" t="s">
-        <v>209</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>83</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E60" t="s">
+        <v>80</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" t="s">
         <v>104</v>
       </c>
-      <c r="B61" t="s">
-        <v>107</v>
-      </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D61" t="s">
-        <v>209</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>83</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B62" t="s">
         <v>19</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>209</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>83</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E62" t="s">
+        <v>80</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D63" t="s">
-        <v>209</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
-        <v>71</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>203</v>
+      </c>
+      <c r="E63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>210</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>133</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E64" t="s">
+        <v>130</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" t="s">
+        <v>130</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
         <v>118</v>
-      </c>
-      <c r="C65" t="s">
-        <v>116</v>
-      </c>
-      <c r="D65" t="s">
-        <v>210</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>133</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" t="s">
-        <v>121</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D66" t="s">
-        <v>210</v>
-      </c>
-      <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>70</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D67" t="s">
-        <v>210</v>
-      </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>133</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E67" t="s">
+        <v>130</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
       </c>
       <c r="C68" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" t="s">
+        <v>204</v>
+      </c>
+      <c r="E68" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" t="s">
         <v>106</v>
       </c>
-      <c r="D68" t="s">
-        <v>210</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68" t="s">
-        <v>72</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>124</v>
-      </c>
-      <c r="B69" t="s">
-        <v>118</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" t="s">
+        <v>130</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" t="s">
         <v>109</v>
       </c>
-      <c r="D69" t="s">
-        <v>210</v>
-      </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D70" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" t="s">
+        <v>130</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
         <v>133</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
-        <v>125</v>
-      </c>
-      <c r="B70" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" t="s">
-        <v>210</v>
-      </c>
-      <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
-        <v>133</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>136</v>
       </c>
       <c r="B71" t="s">
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D71" t="s">
-        <v>210</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71" t="s">
-        <v>133</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E71" t="s">
+        <v>130</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B72" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D72" t="s">
-        <v>210</v>
-      </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72" t="s">
-        <v>133</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E72" t="s">
+        <v>130</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -5212,17 +4977,14 @@
       <c r="D73" t="s">
         <v>4</v>
       </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73" t="s">
-        <v>70</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="E73" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -5235,17 +4997,14 @@
       <c r="D74" t="s">
         <v>4</v>
       </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74" t="s">
-        <v>71</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="E74" t="s">
+        <v>68</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -5255,16 +5014,13 @@
       <c r="C75" t="s">
         <v>10</v>
       </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -5273,21 +5029,18 @@
         <v>10</v>
       </c>
       <c r="D76" t="s">
+        <v>62</v>
+      </c>
+      <c r="E76" t="s">
+        <v>67</v>
+      </c>
+      <c r="F76" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
         <v>64</v>
-      </c>
-      <c r="E76" t="s">
-        <v>10</v>
-      </c>
-      <c r="F76" t="s">
-        <v>70</v>
-      </c>
-      <c r="G76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>66</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -5296,21 +5049,18 @@
         <v>10</v>
       </c>
       <c r="D77" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" t="s">
-        <v>70</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -5319,82 +5069,70 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" t="s">
-        <v>70</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>67</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C79" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D79" t="s">
-        <v>210</v>
-      </c>
-      <c r="E79">
-        <v>2</v>
-      </c>
-      <c r="G79" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="F79" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
         <v>19</v>
       </c>
       <c r="C80" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D80" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80">
-        <v>1</v>
-      </c>
-      <c r="F80" t="s">
-        <v>133</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>204</v>
+      </c>
+      <c r="E80" t="s">
+        <v>130</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D81" t="s">
-        <v>210</v>
-      </c>
-      <c r="E81">
-        <v>1</v>
-      </c>
-      <c r="F81" t="s">
-        <v>133</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>198</v>
+        <v>204</v>
+      </c>
+      <c r="E81" t="s">
+        <v>130</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5405,10 +5143,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5423,251 +5161,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>88</v>
+        <v>130</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>193</v>
-      </c>
-      <c r="E12" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>